<commit_message>
New gap-filled table created
</commit_message>
<xml_diff>
--- a/NeckInj_Uploader.xlsx
+++ b/NeckInj_Uploader.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicko\Documents\GitHub\trackingtables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF98186-EEB7-49CC-985E-36314A3C8F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EB348F-FB01-406C-B120-00BACEBB01FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NeckInj_Uploader" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>LogDate</t>
   </si>
@@ -142,27 +142,6 @@
   </si>
   <si>
     <t>Notes, speech marks added where needed, only when value is not null</t>
-  </si>
-  <si>
-    <t>NO DATA</t>
-  </si>
-  <si>
-    <t>Externality: Fiddling (awkward jobs)</t>
-  </si>
-  <si>
-    <t>Externality: Berry picking</t>
-  </si>
-  <si>
-    <t>Backpack and playing with Amelia</t>
-  </si>
-  <si>
-    <t>Playing with Amelia</t>
-  </si>
-  <si>
-    <t>No UB</t>
-  </si>
-  <si>
-    <t>Forgot Amitriptyline</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2214,11 +2193,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
-    </sheetView>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2263,1432 +2240,576 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C2" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D2" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E2" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A2" s="18"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
-      <c r="H2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
-        <v>2</v>
-      </c>
-      <c r="B3" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C3" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D3" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E3" s="14" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A3" s="18"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
-        <v>3</v>
-      </c>
-      <c r="B4" s="16" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C4" s="16" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D4" s="16" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E4" s="16" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A4" s="19"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="19">
-        <v>4</v>
-      </c>
-      <c r="B5" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C5" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D5" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E5" s="14" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A5" s="19"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
-        <v>5</v>
-      </c>
-      <c r="B6" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C6" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D6" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E6" s="14" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A6" s="19"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
-        <v>6</v>
-      </c>
-      <c r="B7" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C7" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D7" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E7" s="14" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A7" s="19"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
-        <v>7</v>
-      </c>
-      <c r="B8" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C8" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D8" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E8" s="14" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A8" s="19"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
-        <v>8</v>
-      </c>
-      <c r="B9" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C9" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D9" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E9" s="14" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A9" s="19"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
-        <v>9</v>
-      </c>
-      <c r="B10" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C10" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D10" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E10" s="14" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A10" s="19"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
-        <v>10</v>
-      </c>
-      <c r="B11" s="14">
-        <v>2</v>
-      </c>
-      <c r="C11" s="14">
-        <v>1</v>
-      </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="14">
-        <v>0</v>
-      </c>
-      <c r="F11" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G11" s="14" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A11" s="19"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="15"/>
-      <c r="I11" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
-        <v>11</v>
-      </c>
-      <c r="B12" s="14">
-        <v>2</v>
-      </c>
-      <c r="C12" s="14">
-        <v>3</v>
-      </c>
-      <c r="D12" s="14">
-        <v>0</v>
-      </c>
-      <c r="E12" s="14">
-        <v>0</v>
-      </c>
-      <c r="F12" s="14">
-        <v>3</v>
-      </c>
-      <c r="G12" s="14">
-        <v>0</v>
-      </c>
+      <c r="A12" s="19"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
-        <v>12</v>
-      </c>
-      <c r="B13" s="14">
-        <v>2</v>
-      </c>
-      <c r="C13" s="14">
-        <v>2</v>
-      </c>
-      <c r="D13" s="14">
-        <v>0</v>
-      </c>
-      <c r="E13" s="14">
-        <v>0</v>
-      </c>
-      <c r="F13" s="14">
-        <v>3</v>
-      </c>
-      <c r="G13" s="14">
-        <v>3</v>
-      </c>
+      <c r="A13" s="19"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="15"/>
-      <c r="I13" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
-        <v>13</v>
-      </c>
-      <c r="B14" s="14">
-        <v>3</v>
-      </c>
-      <c r="C14" s="14">
-        <v>3</v>
-      </c>
-      <c r="D14" s="15">
-        <v>0</v>
-      </c>
-      <c r="E14" s="15">
-        <v>0</v>
-      </c>
-      <c r="F14" s="15">
-        <v>3</v>
-      </c>
-      <c r="G14" s="15">
-        <v>3</v>
-      </c>
+      <c r="A14" s="19"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
-        <v>14</v>
-      </c>
-      <c r="B15" s="14">
-        <v>2</v>
-      </c>
-      <c r="C15" s="14">
-        <v>3</v>
-      </c>
-      <c r="D15" s="15">
-        <v>0</v>
-      </c>
-      <c r="E15" s="15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="15">
-        <v>3</v>
-      </c>
-      <c r="G15" s="15">
-        <v>3</v>
-      </c>
+      <c r="A15" s="19"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
-        <v>15</v>
-      </c>
-      <c r="B16" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C16" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D16" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E16" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F16" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G16" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A16" s="19"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="15"/>
-      <c r="I16" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
-        <v>16</v>
-      </c>
-      <c r="B17" s="14">
-        <v>3</v>
-      </c>
-      <c r="C17" s="14">
-        <v>3</v>
-      </c>
-      <c r="D17" s="15">
-        <v>0</v>
-      </c>
-      <c r="E17" s="15">
-        <v>0</v>
-      </c>
-      <c r="F17" s="15">
-        <v>3</v>
-      </c>
-      <c r="G17" s="15">
-        <v>4</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="15">
-        <v>-2</v>
-      </c>
+      <c r="A17" s="19"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
-        <v>17</v>
-      </c>
-      <c r="B18" s="14">
-        <v>3</v>
-      </c>
-      <c r="C18" s="14">
-        <v>3</v>
-      </c>
-      <c r="D18" s="14">
-        <v>0</v>
-      </c>
-      <c r="E18" s="14">
-        <v>0</v>
-      </c>
-      <c r="F18" s="15">
-        <v>3</v>
-      </c>
-      <c r="G18" s="15">
-        <v>4</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="15">
-        <v>-2</v>
-      </c>
+      <c r="A18" s="19"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="14">
-        <v>3</v>
-      </c>
-      <c r="C19" s="14">
-        <v>3</v>
-      </c>
-      <c r="D19" s="15">
-        <v>1</v>
-      </c>
-      <c r="E19" s="15">
-        <v>0</v>
-      </c>
-      <c r="F19" s="15">
-        <v>2</v>
-      </c>
-      <c r="G19" s="15">
-        <v>3</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="15">
-        <v>-1</v>
-      </c>
+      <c r="A19" s="19"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
-        <v>19</v>
-      </c>
-      <c r="B20" s="14">
-        <v>2</v>
-      </c>
-      <c r="C20" s="14">
-        <v>3</v>
-      </c>
-      <c r="D20" s="15">
-        <v>0</v>
-      </c>
-      <c r="E20" s="15">
-        <v>0</v>
-      </c>
-      <c r="F20" s="15">
-        <v>2</v>
-      </c>
-      <c r="G20" s="15">
-        <v>3</v>
-      </c>
+      <c r="A20" s="19"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="I20" s="15">
-        <v>0</v>
-      </c>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
-        <v>20</v>
-      </c>
-      <c r="B21" s="14">
-        <v>2</v>
-      </c>
-      <c r="C21" s="14">
-        <v>2</v>
-      </c>
-      <c r="D21" s="15">
-        <v>0</v>
-      </c>
-      <c r="E21" s="15">
-        <v>0</v>
-      </c>
-      <c r="F21" s="15">
-        <v>2</v>
-      </c>
-      <c r="G21" s="15">
-        <v>2</v>
-      </c>
+      <c r="A21" s="19"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
       <c r="H21" s="15"/>
-      <c r="I21" s="15">
-        <v>0</v>
-      </c>
+      <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
-        <v>21</v>
-      </c>
-      <c r="B22" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C22" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D22" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E22" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F22" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G22" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A22" s="19"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
       <c r="H22" s="15"/>
-      <c r="I22" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
-        <v>22</v>
-      </c>
-      <c r="B23" s="14">
-        <v>3</v>
-      </c>
-      <c r="C23" s="14">
-        <v>2</v>
-      </c>
-      <c r="D23" s="15">
-        <v>0</v>
-      </c>
-      <c r="E23" s="15">
-        <v>0</v>
-      </c>
-      <c r="F23" s="15">
-        <v>2</v>
-      </c>
-      <c r="G23" s="15">
-        <v>2</v>
-      </c>
+      <c r="A23" s="19"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="15">
-        <v>0</v>
-      </c>
+      <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
-        <v>23</v>
-      </c>
-      <c r="B24" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C24" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D24" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E24" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F24" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G24" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A24" s="19"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
       <c r="H24" s="15"/>
-      <c r="I24" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="19">
-        <v>24</v>
-      </c>
-      <c r="B25" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C25" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D25" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E25" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F25" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G25" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A25" s="19"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
       <c r="H25" s="15"/>
-      <c r="I25" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I25" s="15"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
-        <v>25</v>
-      </c>
-      <c r="B26" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C26" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D26" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E26" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F26" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G26" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A26" s="19"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
       <c r="H26" s="15"/>
-      <c r="I26" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I26" s="15"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="19">
-        <v>26</v>
-      </c>
-      <c r="B27" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C27" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D27" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E27" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F27" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G27" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A27" s="19"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I27" s="15"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
-        <v>27</v>
-      </c>
-      <c r="B28" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C28" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D28" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E28" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F28" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G28" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A28" s="19"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="19">
-        <v>28</v>
-      </c>
-      <c r="B29" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C29" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D29" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E29" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F29" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G29" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A29" s="19"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="19">
-        <v>29</v>
-      </c>
-      <c r="B30" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C30" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D30" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E30" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F30" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G30" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A30" s="19"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
       <c r="H30" s="15"/>
-      <c r="I30" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
-        <v>30</v>
-      </c>
-      <c r="B31" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C31" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D31" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E31" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F31" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G31" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A31" s="19"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
       <c r="H31" s="15"/>
-      <c r="I31" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
-        <v>31</v>
-      </c>
-      <c r="B32" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C32" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D32" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E32" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F32" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G32" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A32" s="19"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
       <c r="H32" s="15"/>
-      <c r="I32" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="19">
-        <v>32</v>
-      </c>
-      <c r="B33" s="14">
-        <v>2</v>
-      </c>
-      <c r="C33" s="14">
-        <v>1</v>
-      </c>
-      <c r="D33" s="14">
-        <v>0</v>
-      </c>
-      <c r="E33" s="14">
-        <v>0</v>
-      </c>
-      <c r="F33" s="15">
-        <v>1</v>
-      </c>
-      <c r="G33" s="15">
-        <v>0</v>
-      </c>
+      <c r="A33" s="19"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
       <c r="H33" s="15"/>
-      <c r="I33" s="15">
-        <v>0</v>
-      </c>
+      <c r="I33" s="15"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="19">
-        <v>33</v>
-      </c>
-      <c r="B34" s="14">
-        <v>1</v>
-      </c>
-      <c r="C34" s="14">
-        <v>1</v>
-      </c>
-      <c r="D34" s="14">
-        <v>0</v>
-      </c>
-      <c r="E34" s="14">
-        <v>0</v>
-      </c>
-      <c r="F34" s="15">
-        <v>1</v>
-      </c>
-      <c r="G34" s="15">
-        <v>1</v>
-      </c>
+      <c r="A34" s="19"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
       <c r="H34" s="17"/>
-      <c r="I34" s="15">
-        <v>0</v>
-      </c>
+      <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="19">
-        <v>34</v>
-      </c>
-      <c r="B35" s="14">
-        <v>1</v>
-      </c>
-      <c r="C35" s="14">
-        <v>1</v>
-      </c>
-      <c r="D35" s="14">
-        <v>0</v>
-      </c>
-      <c r="E35" s="14">
-        <v>0</v>
-      </c>
-      <c r="F35" s="15">
-        <v>1</v>
-      </c>
-      <c r="G35" s="15">
-        <v>1</v>
-      </c>
+      <c r="A35" s="19"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
       <c r="H35" s="15"/>
-      <c r="I35" s="15">
-        <v>0</v>
-      </c>
+      <c r="I35" s="15"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="19">
-        <v>35</v>
-      </c>
-      <c r="B36" s="14">
-        <v>1</v>
-      </c>
-      <c r="C36" s="14">
-        <v>1</v>
-      </c>
-      <c r="D36" s="14">
-        <v>2</v>
-      </c>
-      <c r="E36" s="14">
-        <v>2</v>
-      </c>
-      <c r="F36" s="15">
-        <v>1</v>
-      </c>
-      <c r="G36" s="15">
-        <v>1</v>
-      </c>
+      <c r="A36" s="19"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
       <c r="H36" s="15"/>
-      <c r="I36" s="15">
-        <v>0</v>
-      </c>
+      <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="19">
-        <v>36</v>
-      </c>
-      <c r="B37" s="14">
-        <v>2</v>
-      </c>
-      <c r="C37" s="14">
-        <v>1</v>
-      </c>
-      <c r="D37" s="14">
-        <v>0</v>
-      </c>
-      <c r="E37" s="14">
-        <v>0</v>
-      </c>
-      <c r="F37" s="15">
-        <v>1</v>
-      </c>
-      <c r="G37" s="15">
-        <v>1</v>
-      </c>
+      <c r="A37" s="19"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
       <c r="H37" s="15"/>
-      <c r="I37" s="15">
-        <v>0</v>
-      </c>
+      <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="19">
-        <v>37</v>
-      </c>
-      <c r="B38" s="14">
-        <v>2</v>
-      </c>
-      <c r="C38" s="14">
-        <v>2</v>
-      </c>
-      <c r="D38" s="14">
-        <v>0</v>
-      </c>
-      <c r="E38" s="14">
-        <v>0</v>
-      </c>
-      <c r="F38" s="15">
-        <v>1</v>
-      </c>
-      <c r="G38" s="15">
-        <v>1</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="15">
-        <v>-1</v>
-      </c>
+      <c r="A38" s="19"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="19">
-        <v>38</v>
-      </c>
-      <c r="B39" s="14">
-        <v>2</v>
-      </c>
-      <c r="C39" s="14">
-        <v>2</v>
-      </c>
-      <c r="D39" s="14">
-        <v>0</v>
-      </c>
-      <c r="E39" s="14">
-        <v>0</v>
-      </c>
-      <c r="F39" s="15">
-        <v>2</v>
-      </c>
-      <c r="G39" s="15">
-        <v>2</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" s="15">
-        <v>-1</v>
-      </c>
+      <c r="A39" s="19"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="19">
-        <v>39</v>
-      </c>
-      <c r="B40" s="14">
-        <v>2</v>
-      </c>
-      <c r="C40" s="14">
-        <v>2</v>
-      </c>
-      <c r="D40" s="14">
-        <v>0</v>
-      </c>
-      <c r="E40" s="14">
-        <v>0</v>
-      </c>
-      <c r="F40" s="15">
-        <v>1</v>
-      </c>
-      <c r="G40" s="15">
-        <v>2</v>
-      </c>
+      <c r="A40" s="19"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
       <c r="H40" s="15"/>
-      <c r="I40" s="15">
-        <v>0</v>
-      </c>
+      <c r="I40" s="15"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="19">
-        <v>40</v>
-      </c>
-      <c r="B41" s="14">
-        <v>3</v>
-      </c>
-      <c r="C41" s="14">
-        <v>2</v>
-      </c>
-      <c r="D41" s="14">
-        <v>0</v>
-      </c>
-      <c r="E41" s="14">
-        <v>0</v>
-      </c>
-      <c r="F41" s="15">
-        <v>1</v>
-      </c>
-      <c r="G41" s="15">
-        <v>2</v>
-      </c>
+      <c r="A41" s="19"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
       <c r="H41" s="15"/>
-      <c r="I41" s="15">
-        <v>0</v>
-      </c>
+      <c r="I41" s="15"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="19">
-        <v>41</v>
-      </c>
-      <c r="B42" s="14">
-        <v>2</v>
-      </c>
-      <c r="C42" s="14">
-        <v>3</v>
-      </c>
-      <c r="D42" s="14">
-        <v>0</v>
-      </c>
-      <c r="E42" s="14">
-        <v>0</v>
-      </c>
-      <c r="F42" s="15">
-        <v>1</v>
-      </c>
-      <c r="G42" s="15">
-        <v>3</v>
-      </c>
+      <c r="A42" s="19"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
       <c r="H42" s="15"/>
-      <c r="I42" s="15">
-        <v>0</v>
-      </c>
+      <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="19">
-        <v>42</v>
-      </c>
-      <c r="B43" s="14">
-        <v>2</v>
-      </c>
-      <c r="C43" s="14">
-        <v>3</v>
-      </c>
-      <c r="D43" s="14">
-        <v>0</v>
-      </c>
-      <c r="E43" s="14">
-        <v>0</v>
-      </c>
-      <c r="F43" s="15">
-        <v>1</v>
-      </c>
-      <c r="G43" s="15">
-        <v>3</v>
-      </c>
+      <c r="A43" s="19"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
       <c r="H43" s="15"/>
-      <c r="I43" s="15">
-        <v>0</v>
-      </c>
+      <c r="I43" s="15"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="19">
-        <v>43</v>
-      </c>
-      <c r="B44" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C44" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D44" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E44" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F44" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G44" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H44" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I44" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A44" s="19"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="19">
-        <v>44</v>
-      </c>
-      <c r="B45" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C45" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D45" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E45" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F45" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G45" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H45" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I45" s="15" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A45" s="19"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="19">
-        <v>45</v>
-      </c>
-      <c r="B46" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C46" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D46" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E46" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F46" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G46" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H46" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I46" s="14" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A46" s="19"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="19">
-        <v>46</v>
-      </c>
-      <c r="B47" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C47" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D47" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E47" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F47" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G47" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H47" s="14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I47" s="14" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A47" s="19"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="19">
-        <v>47</v>
-      </c>
-      <c r="B48" s="14">
-        <v>2</v>
-      </c>
-      <c r="C48" s="14">
-        <v>3</v>
-      </c>
-      <c r="D48" s="14">
-        <v>0</v>
-      </c>
-      <c r="E48" s="14">
-        <v>0</v>
-      </c>
-      <c r="F48" s="14">
-        <v>1</v>
-      </c>
-      <c r="G48" s="14">
-        <v>2</v>
-      </c>
+      <c r="A48" s="19"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
       <c r="H48" s="14"/>
-      <c r="I48" s="14">
-        <v>0</v>
-      </c>
+      <c r="I48" s="14"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="19">
-        <v>48</v>
-      </c>
-      <c r="B49" s="14">
-        <v>2</v>
-      </c>
-      <c r="C49" s="14">
-        <v>3</v>
-      </c>
-      <c r="D49" s="14">
-        <v>0</v>
-      </c>
-      <c r="E49" s="14">
-        <v>0</v>
-      </c>
-      <c r="F49" s="14">
-        <v>2</v>
-      </c>
-      <c r="G49" s="14">
-        <v>2</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I49" s="14">
-        <v>-1</v>
-      </c>
+      <c r="A49" s="19"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="19">
-        <v>49</v>
-      </c>
-      <c r="B50" s="14">
-        <v>1</v>
-      </c>
-      <c r="C50" s="14">
-        <v>2</v>
-      </c>
-      <c r="D50" s="14">
-        <v>0</v>
-      </c>
-      <c r="E50" s="14">
-        <v>0</v>
-      </c>
-      <c r="F50" s="15">
-        <v>1</v>
-      </c>
-      <c r="G50" s="15">
-        <v>2</v>
-      </c>
+      <c r="A50" s="19"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
       <c r="H50" s="15"/>
-      <c r="I50" s="15">
-        <v>0</v>
-      </c>
+      <c r="I50" s="15"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="19">
-        <v>50</v>
-      </c>
-      <c r="B51" s="14">
-        <v>2</v>
-      </c>
-      <c r="C51" s="14">
-        <v>2</v>
-      </c>
-      <c r="D51" s="14">
-        <v>0</v>
-      </c>
-      <c r="E51" s="14">
-        <v>0</v>
-      </c>
-      <c r="F51" s="15">
-        <v>2</v>
-      </c>
-      <c r="G51" s="15">
-        <v>0</v>
-      </c>
+      <c r="A51" s="19"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
       <c r="H51" s="15"/>
-      <c r="I51" s="15">
-        <v>0</v>
-      </c>
+      <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="19">
-        <v>51</v>
-      </c>
-      <c r="B52" s="14">
-        <v>2</v>
-      </c>
-      <c r="C52" s="14">
-        <v>2</v>
-      </c>
-      <c r="D52" s="14">
-        <v>0</v>
-      </c>
-      <c r="E52" s="14">
-        <v>0</v>
-      </c>
-      <c r="F52" s="15">
-        <v>1</v>
-      </c>
-      <c r="G52" s="15">
-        <v>0</v>
-      </c>
-      <c r="H52" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="A52" s="19"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
       <c r="I52" s="15"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="19">
-        <v>52</v>
-      </c>
-      <c r="B53" s="14">
-        <v>1</v>
-      </c>
-      <c r="C53" s="14">
-        <v>2</v>
-      </c>
-      <c r="D53" s="14">
-        <v>0</v>
-      </c>
-      <c r="E53" s="14">
-        <v>0</v>
-      </c>
-      <c r="F53" s="15">
-        <v>1</v>
-      </c>
-      <c r="G53" s="15">
-        <v>0</v>
-      </c>
+      <c r="A53" s="19"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
       <c r="H53" s="15"/>
-      <c r="I53" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="19"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
+      <c r="I53" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploader finished for latest table format
</commit_message>
<xml_diff>
--- a/NeckInj_Uploader.xlsx
+++ b/NeckInj_Uploader.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicko\Documents\GitHub\trackingtables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EB348F-FB01-406C-B120-00BACEBB01FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7509836D-4BB8-4512-ADEC-FA29F6CE330E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NeckInj_Uploader" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>LogDate</t>
   </si>
@@ -121,20 +121,6 @@
     <t>ExternalityAdjustment</t>
   </si>
   <si>
-    <t>INSERT INTO dbo.NeckInj (
-	LogDate,
-	RightPain,
-	RightNumb,
-	LeftPain,
-	LeftNumb,
-	LeftElbowPain,
-	LeftElbowNumb,
-	Notes,
-	ExternalityAdjustment
-)
-VALUES</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -142,6 +128,27 @@
   </si>
   <si>
     <t>Notes, speech marks added where needed, only when value is not null</t>
+  </si>
+  <si>
+    <t>PeriodName</t>
+  </si>
+  <si>
+    <t>PeriodName, speech marks added where needed, only when value is not null</t>
+  </si>
+  <si>
+    <t>INSERT INTO dbo.NeckInj_wPeriod (
+	LogDate,
+	LeftPain,
+	LeftNumb,
+	RightPain,
+	RightNumb,
+	LeftElbowPain,
+	LeftElbowNumb,
+	Notes,
+	ExternalityAdjustment,
+                PeriodName
+)
+VALUES</t>
   </si>
 </sst>
 </file>
@@ -1106,40 +1113,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="63.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="39.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="63.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>5</v>
@@ -1153,14 +1160,20 @@
       <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1170,16 +1183,12 @@
       <c r="G2" s="10"/>
       <c r="H2" s="5"/>
       <c r="I2" s="10"/>
-      <c r="J2" s="8" t="str">
-        <f>IF(H2="NULL","NULL",CONCATENATE(CHAR(39),H2,CHAR(39)))</f>
-        <v>''</v>
-      </c>
-      <c r="K2" s="8" t="str">
-        <f>"('"&amp;A2&amp;"',"&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;","&amp;J2&amp;","&amp;I2&amp;"),"</f>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="10"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1189,16 +1198,12 @@
       <c r="G3" s="10"/>
       <c r="H3" s="5"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="8" t="str">
-        <f t="shared" ref="J3:J55" si="0">IF(H3="NULL","NULL",CONCATENATE(CHAR(39),H3,CHAR(39)))</f>
-        <v>''</v>
-      </c>
-      <c r="K3" s="8" t="str">
-        <f t="shared" ref="K3:K55" si="1">"('"&amp;A3&amp;"',"&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;J3&amp;","&amp;I3&amp;"),"</f>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J3" s="10"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1208,16 +1213,12 @@
       <c r="G4" s="10"/>
       <c r="H4" s="5"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K4" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="10"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1227,16 +1228,12 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K5" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="10"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1246,16 +1243,12 @@
       <c r="G6" s="10"/>
       <c r="H6" s="5"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K6" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" s="10"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1265,16 +1258,12 @@
       <c r="G7" s="10"/>
       <c r="H7" s="5"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K7" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="10"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1284,16 +1273,12 @@
       <c r="G8" s="10"/>
       <c r="H8" s="5"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K8" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="10"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1303,16 +1288,12 @@
       <c r="G9" s="10"/>
       <c r="H9" s="5"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K9" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="10"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1322,16 +1303,12 @@
       <c r="G10" s="10"/>
       <c r="H10" s="5"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K10" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="10"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1341,16 +1318,12 @@
       <c r="G11" s="10"/>
       <c r="H11" s="5"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K11" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="10"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1360,831 +1333,10 @@
       <c r="G12" s="10"/>
       <c r="H12" s="5"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K12" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K13" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K14" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K15" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K16" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K17" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K18" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K19" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K20" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K21" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K22" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K23" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K24" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K25" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K26" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K27" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K28" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K29" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K30" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K31" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K32" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K33" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K34" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K35" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K36" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K37" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K38" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K39" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K40" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K41" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K42" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K43" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K44" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K45" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K46" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K47" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K48" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K49" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K50" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K51" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K52" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K53" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="10"/>
-      <c r="J54" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K54" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>''</v>
-      </c>
-      <c r="K55" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>('',,,,,,,'',),</v>
-      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2193,38 +1345,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>5</v>
@@ -2236,21 +1389,25 @@
         <v>7</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -2260,9 +1417,10 @@
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="J3" s="15"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -2271,20 +1429,22 @@
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
+      <c r="H5" s="14"/>
       <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -2293,9 +1453,10 @@
       <c r="G6" s="14"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2304,9 +1465,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -2315,9 +1477,10 @@
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -2326,9 +1489,10 @@
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -2337,9 +1501,10 @@
       <c r="G10" s="14"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -2348,20 +1513,22 @@
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
+      <c r="H12" s="14"/>
       <c r="I12" s="15"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -2370,52 +1537,57 @@
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -2425,63 +1597,69 @@
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="15"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="15"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="15"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -2491,8 +1669,9 @@
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="15"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -2502,8 +1681,9 @@
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="15"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -2513,8 +1693,9 @@
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="15"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -2524,8 +1705,9 @@
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -2535,8 +1717,9 @@
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="15"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -2546,8 +1729,9 @@
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -2557,8 +1741,9 @@
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="15"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -2568,8 +1753,9 @@
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="15"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -2579,8 +1765,9 @@
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="15"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -2590,8 +1777,9 @@
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -2601,8 +1789,9 @@
       <c r="G34" s="15"/>
       <c r="H34" s="17"/>
       <c r="I34" s="15"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="15"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -2612,8 +1801,9 @@
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="15"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -2623,8 +1813,9 @@
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="15"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -2634,8 +1825,9 @@
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="15"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -2645,8 +1837,9 @@
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="15"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -2656,8 +1849,9 @@
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="15"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -2667,8 +1861,9 @@
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="15"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -2678,8 +1873,9 @@
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="15"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -2689,8 +1885,9 @@
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="15"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -2700,8 +1897,9 @@
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="15"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -2711,8 +1909,9 @@
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
       <c r="I44" s="15"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="15"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -2722,8 +1921,9 @@
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="15"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -2733,8 +1933,9 @@
       <c r="G46" s="14"/>
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="14"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -2744,8 +1945,9 @@
       <c r="G47" s="14"/>
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="14"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -2755,8 +1957,9 @@
       <c r="G48" s="14"/>
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="14"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -2766,8 +1969,9 @@
       <c r="G49" s="14"/>
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="14"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="19"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -2777,8 +1981,9 @@
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="15"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -2788,8 +1993,9 @@
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="15"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="19"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -2799,8 +2005,9 @@
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
       <c r="I52" s="15"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="15"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="19"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -2810,6 +2017,7 @@
       <c r="G53" s="15"/>
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor mistakes fixed in uploaded
</commit_message>
<xml_diff>
--- a/NeckInj_Uploader.xlsx
+++ b/NeckInj_Uploader.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicko\Documents\GitHub\trackingtables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7509836D-4BB8-4512-ADEC-FA29F6CE330E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41876C01-8881-4EF1-B05D-E4C086792D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NeckInj_Uploader" sheetId="1" r:id="rId1"/>
@@ -749,15 +749,13 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1113,9 +1111,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1125,9 +1123,9 @@
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="39.7109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="63.5703125" style="3" customWidth="1"/>
   </cols>
@@ -1338,6 +1336,131 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+    </row>
+    <row r="24" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+    </row>
+    <row r="28" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+    </row>
+    <row r="29" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+    </row>
+    <row r="30" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+    </row>
+    <row r="31" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+    </row>
+    <row r="32" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+    </row>
+    <row r="34" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+    </row>
+    <row r="35" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+    </row>
+    <row r="36" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+    </row>
+    <row r="37" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1345,9 +1468,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1361,6 +1484,7 @@
     <col min="8" max="8" width="31.28515625" customWidth="1"/>
     <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
@@ -1396,7 +1520,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="14"/>
@@ -1408,7 +1532,7 @@
       <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -1420,7 +1544,7 @@
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -1432,7 +1556,7 @@
       <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1444,7 +1568,7 @@
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -1456,7 +1580,7 @@
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1468,7 +1592,7 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -1480,7 +1604,7 @@
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -1492,7 +1616,7 @@
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -1504,7 +1628,7 @@
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1516,7 +1640,7 @@
       <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -1528,7 +1652,7 @@
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1540,7 +1664,7 @@
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="14"/>
@@ -1552,7 +1676,7 @@
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="14"/>
@@ -1564,7 +1688,7 @@
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="14"/>
@@ -1575,8 +1699,8 @@
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
@@ -1587,8 +1711,8 @@
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -1598,9 +1722,10 @@
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="L18" s="19"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="14"/>
@@ -1610,9 +1735,10 @@
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="L19" s="19"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
@@ -1623,8 +1749,8 @@
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="14"/>
@@ -1635,8 +1761,8 @@
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="14"/>
@@ -1647,8 +1773,8 @@
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="14"/>
@@ -1659,8 +1785,8 @@
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
@@ -1671,8 +1797,8 @@
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
@@ -1683,8 +1809,8 @@
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
@@ -1695,8 +1821,8 @@
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -1707,8 +1833,8 @@
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
@@ -1719,8 +1845,8 @@
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
@@ -1731,8 +1857,8 @@
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
@@ -1743,8 +1869,8 @@
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
@@ -1755,8 +1881,8 @@
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
@@ -1768,7 +1894,7 @@
       <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
@@ -1780,19 +1906,19 @@
       <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
-      <c r="H34" s="17"/>
+      <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
       <c r="D35" s="14"/>
@@ -1804,7 +1930,7 @@
       <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
@@ -1816,7 +1942,7 @@
       <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>
@@ -1828,7 +1954,7 @@
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
       <c r="D38" s="14"/>
@@ -1840,7 +1966,7 @@
       <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
@@ -1852,7 +1978,7 @@
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
@@ -1864,7 +1990,7 @@
       <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
@@ -1876,7 +2002,7 @@
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
@@ -1888,7 +2014,7 @@
       <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
@@ -1900,7 +2026,7 @@
       <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
@@ -1912,7 +2038,7 @@
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
@@ -1924,7 +2050,7 @@
       <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
       <c r="D46" s="14"/>
@@ -1936,7 +2062,7 @@
       <c r="J46" s="14"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
+      <c r="A47" s="18"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
       <c r="D47" s="14"/>
@@ -1948,7 +2074,7 @@
       <c r="J47" s="14"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
+      <c r="A48" s="18"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
@@ -1960,7 +2086,7 @@
       <c r="J48" s="14"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
+      <c r="A49" s="18"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
@@ -1972,7 +2098,7 @@
       <c r="J49" s="14"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
+      <c r="A50" s="18"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
@@ -1984,7 +2110,7 @@
       <c r="J50" s="15"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
+      <c r="A51" s="18"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
@@ -1996,7 +2122,7 @@
       <c r="J51" s="15"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
@@ -2008,7 +2134,7 @@
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>

</xml_diff>

<commit_message>
Fix missing column formulae in uploaders
</commit_message>
<xml_diff>
--- a/NeckInj_Uploader.xlsx
+++ b/NeckInj_Uploader.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicko\Documents\GitHub\trackingtables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41876C01-8881-4EF1-B05D-E4C086792D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDFB796-291D-4C7B-BECE-29CC4C6AB942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NeckInj_Uploader" sheetId="1" r:id="rId1"/>
@@ -1113,19 +1113,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="39.7109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="63.5703125" style="3" customWidth="1"/>
   </cols>
@@ -1182,9 +1184,18 @@
       <c r="H2" s="5"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="K2" s="8" t="str">
+        <f>IF(ISBLANK(H2),"","'"&amp;H2&amp;"'")</f>
+        <v/>
+      </c>
+      <c r="L2" s="8" t="str">
+        <f>IF(ISBLANK(J2),"","'"&amp;J2&amp;"'")</f>
+        <v/>
+      </c>
+      <c r="M2" s="8" t="str">
+        <f>A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;G2&amp;", "&amp;K2&amp;", "&amp;I2&amp;", "&amp;L2</f>
+        <v xml:space="preserve">, , , , , , , , , </v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -1197,9 +1208,18 @@
       <c r="H3" s="5"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="K3" s="8" t="str">
+        <f t="shared" ref="K3:K12" si="0">IF(ISBLANK(H3),"","'"&amp;H3&amp;"'")</f>
+        <v/>
+      </c>
+      <c r="L3" s="8" t="str">
+        <f t="shared" ref="L3:L12" si="1">IF(ISBLANK(J3),"","'"&amp;J3&amp;"'")</f>
+        <v/>
+      </c>
+      <c r="M3" s="8" t="str">
+        <f t="shared" ref="M3:M12" si="2">A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;", "&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;", "&amp;K3&amp;", "&amp;I3&amp;", "&amp;L3</f>
+        <v xml:space="preserve">, , , , , , , , , </v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
@@ -1212,9 +1232,18 @@
       <c r="H4" s="5"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="K4" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L4" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M4" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">, , , , , , , , , </v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
@@ -1227,9 +1256,18 @@
       <c r="H5" s="5"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="K5" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L5" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M5" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">, , , , , , , , , </v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
@@ -1242,9 +1280,18 @@
       <c r="H6" s="5"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="K6" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L6" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M6" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">, , , , , , , , , </v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -1257,9 +1304,18 @@
       <c r="H7" s="5"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="K7" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M7" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">, , , , , , , , , </v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
@@ -1272,9 +1328,18 @@
       <c r="H8" s="5"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="K8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L8" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">, , , , , , , , , </v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -1287,9 +1352,18 @@
       <c r="H9" s="5"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
+      <c r="K9" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L9" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">, , , , , , , , , </v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
@@ -1302,9 +1376,18 @@
       <c r="H10" s="5"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
+      <c r="K10" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L10" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M10" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">, , , , , , , , , </v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
@@ -1317,9 +1400,18 @@
       <c r="H11" s="5"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="K11" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L11" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M11" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">, , , , , , , , , </v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
@@ -1332,9 +1424,18 @@
       <c r="H12" s="5"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
+      <c r="K12" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L12" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M12" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">, , , , , , , , , </v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K13" s="8"/>

</xml_diff>

<commit_message>
SQL and Raw Excel imported
Next step: Finish excel importer by processing data into required format for SQL upload
</commit_message>
<xml_diff>
--- a/NeckInj_Uploader.xlsx
+++ b/NeckInj_Uploader.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicko\Documents\GitHub\trackingtables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDFB796-291D-4C7B-BECE-29CC4C6AB942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EB27B5-65FD-4DAE-B61E-9721AE5AA919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="NeckInj_Uploader" sheetId="1" r:id="rId1"/>
-    <sheet name="Scratch_Formatter" sheetId="3" r:id="rId2"/>
+    <sheet name="Scratch_Formatter" sheetId="3" r:id="rId1"/>
+    <sheet name="NeckInj_Uploader" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,66 +33,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Nick Collis</author>
-  </authors>
-  <commentList>
-    <comment ref="I46" authorId="0" shapeId="0" xr:uid="{FE9F1A43-765F-4746-9355-639641945E4C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nick Collis:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Effect of previous two days winding down.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I50" authorId="0" shapeId="0" xr:uid="{5F3BF56B-D981-4334-862B-49A3F20C003B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nick Collis:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Didn't take amitriptyline the day before.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>LogDate</t>
   </si>
@@ -150,6 +92,21 @@
 )
 VALUES</t>
   </si>
+  <si>
+    <t>No Externalities</t>
+  </si>
+  <si>
+    <t>Mid 2022 Start</t>
+  </si>
+  <si>
+    <t>Side lying in bed</t>
+  </si>
+  <si>
+    <t>Moving bags of cement</t>
+  </si>
+  <si>
+    <t>No exercise</t>
+  </si>
 </sst>
 </file>
 
@@ -158,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,19 +257,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="36">
@@ -715,7 +659,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -750,9 +694,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1110,10 +1051,552 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>44864</v>
+      </c>
+      <c r="B2" s="15">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14">
+        <v>1</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>44874</v>
+      </c>
+      <c r="B3" s="14">
+        <v>3</v>
+      </c>
+      <c r="C3" s="14">
+        <v>3</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>44875</v>
+      </c>
+      <c r="B4" s="16">
+        <v>2</v>
+      </c>
+      <c r="C4" s="16">
+        <v>3</v>
+      </c>
+      <c r="D4" s="16">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16">
+        <v>1</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>44876</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>44877</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14">
+        <v>2</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>44878</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2</v>
+      </c>
+      <c r="C7" s="14">
+        <v>2</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>44879</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>44880</v>
+      </c>
+      <c r="B9" s="14">
+        <v>2</v>
+      </c>
+      <c r="C9" s="14">
+        <v>2</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>44881</v>
+      </c>
+      <c r="B10" s="14">
+        <v>2</v>
+      </c>
+      <c r="C10" s="14">
+        <v>2</v>
+      </c>
+      <c r="D10" s="14">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>44882</v>
+      </c>
+      <c r="B11" s="14">
+        <v>2</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>44883</v>
+      </c>
+      <c r="B12" s="14">
+        <v>2</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
+        <v>44884</v>
+      </c>
+      <c r="B13" s="14">
+        <v>1</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>44885</v>
+      </c>
+      <c r="B14" s="15">
+        <v>1</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>44886</v>
+      </c>
+      <c r="B15" s="15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="14">
+        <v>1</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
+        <v>44887</v>
+      </c>
+      <c r="B16" s="15">
+        <v>3</v>
+      </c>
+      <c r="C16" s="15">
+        <v>3</v>
+      </c>
+      <c r="D16" s="14">
+        <v>0</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>44888</v>
+      </c>
+      <c r="B17" s="15">
+        <v>2</v>
+      </c>
+      <c r="C17" s="15">
+        <v>2</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1</v>
+      </c>
+      <c r="E17" s="14">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>44889</v>
+      </c>
+      <c r="B18" s="14">
+        <v>2</v>
+      </c>
+      <c r="C18" s="14">
+        <v>2</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>44890</v>
+      </c>
+      <c r="B19" s="15">
+        <v>2</v>
+      </c>
+      <c r="C19" s="15">
+        <v>2</v>
+      </c>
+      <c r="D19" s="14">
+        <v>1</v>
+      </c>
+      <c r="E19" s="14">
+        <v>1</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="L19" s="18"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>44891</v>
+      </c>
+      <c r="B20" s="15">
+        <v>1</v>
+      </c>
+      <c r="C20" s="15">
+        <v>1</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0</v>
+      </c>
+      <c r="E20" s="14">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>44892</v>
+      </c>
+      <c r="B21" s="15">
+        <v>3</v>
+      </c>
+      <c r="C21" s="15">
+        <v>3</v>
+      </c>
+      <c r="D21" s="14">
+        <v>0</v>
+      </c>
+      <c r="E21" s="14">
+        <v>2</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1565,689 +2048,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L53"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.28515625" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="L18" s="19"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="L19" s="19"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="15"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>